<commit_message>
added postag results ws.
</commit_message>
<xml_diff>
--- a/output/TTTT.xlsx
+++ b/output/TTTT.xlsx
@@ -1,29 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pree\Thai_SA_journal\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD6DE942-A2BE-435F-8AB4-CE2B6E8C00B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E223C03D-CFD3-4A6D-90EE-024811127DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{9BDD03C8-F7C5-4674-9603-EB57B3FD651B}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="5" activeTab="14" xr2:uid="{9BDD03C8-F7C5-4674-9603-EB57B3FD651B}"/>
   </bookViews>
   <sheets>
     <sheet name="BOW1" sheetId="1" r:id="rId1"/>
-    <sheet name="TFIDF1" sheetId="2" r:id="rId2"/>
-    <sheet name="BOW12" sheetId="9" r:id="rId3"/>
-    <sheet name="TFIDF12" sheetId="10" r:id="rId4"/>
-    <sheet name="BOW2" sheetId="3" r:id="rId5"/>
-    <sheet name="TFIDF2" sheetId="4" r:id="rId6"/>
-    <sheet name="DICTBOW" sheetId="5" r:id="rId7"/>
-    <sheet name="DICTTFIDF" sheetId="6" r:id="rId8"/>
-    <sheet name="W2V_AVG" sheetId="8" r:id="rId9"/>
-    <sheet name="W2V_TF" sheetId="11" r:id="rId10"/>
-    <sheet name="POSTAG" sheetId="7" r:id="rId11"/>
+    <sheet name="Sheet1" sheetId="12" r:id="rId2"/>
+    <sheet name="TFIDF1" sheetId="2" r:id="rId3"/>
+    <sheet name="BOW12" sheetId="9" r:id="rId4"/>
+    <sheet name="TFIDF12" sheetId="10" r:id="rId5"/>
+    <sheet name="BOW2" sheetId="3" r:id="rId6"/>
+    <sheet name="TFIDF2" sheetId="4" r:id="rId7"/>
+    <sheet name="DICTBOW" sheetId="5" r:id="rId8"/>
+    <sheet name="DICTTFIDF" sheetId="6" r:id="rId9"/>
+    <sheet name="W2V_AVG" sheetId="8" r:id="rId10"/>
+    <sheet name="W2V_TF" sheetId="11" r:id="rId11"/>
+    <sheet name="POSTAG-BOW" sheetId="7" r:id="rId12"/>
+    <sheet name="POSTAG-AVG" sheetId="13" r:id="rId13"/>
+    <sheet name="POSTAG-CONCAT" sheetId="14" r:id="rId14"/>
+    <sheet name="POSTAG-FLAT" sheetId="15" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1726" uniqueCount="1354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1804" uniqueCount="1354">
   <si>
     <t>SVM</t>
   </si>
@@ -4488,7 +4492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDE8EA2A-9E9F-440E-AA8B-BE5295D9DA09}">
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
@@ -5073,6 +5077,559 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E672E80F-B107-465D-99B6-B0D1191F61A9}">
+  <dimension ref="A1:N14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="7" customFormat="1">
+      <c r="A3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>1126</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>1127</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>1128</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>1129</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>1130</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>1131</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>1132</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>1133</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>1134</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>1135</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>873</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1136</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1137</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1138</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1139</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1140</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1141</v>
+      </c>
+      <c r="J4" t="s">
+        <v>1142</v>
+      </c>
+      <c r="K4" t="s">
+        <v>72</v>
+      </c>
+      <c r="L4" t="s">
+        <v>1143</v>
+      </c>
+      <c r="M4" t="s">
+        <v>1144</v>
+      </c>
+      <c r="N4" t="s">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1146</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1147</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1148</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1149</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1150</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1151</v>
+      </c>
+      <c r="I5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J5" t="s">
+        <v>85</v>
+      </c>
+      <c r="K5" t="s">
+        <v>1152</v>
+      </c>
+      <c r="L5" t="s">
+        <v>1153</v>
+      </c>
+      <c r="M5" t="s">
+        <v>1154</v>
+      </c>
+      <c r="N5" t="s">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1156</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1157</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1158</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1159</v>
+      </c>
+      <c r="F6" t="s">
+        <v>148</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1160</v>
+      </c>
+      <c r="I6" t="s">
+        <v>444</v>
+      </c>
+      <c r="J6" t="s">
+        <v>1161</v>
+      </c>
+      <c r="K6" t="s">
+        <v>1162</v>
+      </c>
+      <c r="L6" t="s">
+        <v>1163</v>
+      </c>
+      <c r="M6" t="s">
+        <v>1164</v>
+      </c>
+      <c r="N6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1166</v>
+      </c>
+      <c r="D7" t="s">
+        <v>551</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1167</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1168</v>
+      </c>
+      <c r="G7" t="s">
+        <v>1169</v>
+      </c>
+      <c r="I7" t="s">
+        <v>925</v>
+      </c>
+      <c r="J7" t="s">
+        <v>1170</v>
+      </c>
+      <c r="K7" t="s">
+        <v>1171</v>
+      </c>
+      <c r="L7" t="s">
+        <v>1172</v>
+      </c>
+      <c r="M7" t="s">
+        <v>78</v>
+      </c>
+      <c r="N7" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="5" customFormat="1">
+      <c r="A8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>1173</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>1174</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>1176</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>1177</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>1178</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>1179</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>1180</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>1181</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>1182</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1183</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1184</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1185</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F9" t="s">
+        <v>628</v>
+      </c>
+      <c r="G9" t="s">
+        <v>1187</v>
+      </c>
+      <c r="I9" t="s">
+        <v>1188</v>
+      </c>
+      <c r="J9" t="s">
+        <v>1189</v>
+      </c>
+      <c r="K9" t="s">
+        <v>1190</v>
+      </c>
+      <c r="L9" t="s">
+        <v>1191</v>
+      </c>
+      <c r="M9" t="s">
+        <v>1192</v>
+      </c>
+      <c r="N9" t="s">
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1194</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1195</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1196</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1197</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1198</v>
+      </c>
+      <c r="G10" t="s">
+        <v>1199</v>
+      </c>
+      <c r="I10" t="s">
+        <v>1200</v>
+      </c>
+      <c r="J10" t="s">
+        <v>41</v>
+      </c>
+      <c r="K10" t="s">
+        <v>1201</v>
+      </c>
+      <c r="L10" t="s">
+        <v>1202</v>
+      </c>
+      <c r="M10" t="s">
+        <v>1203</v>
+      </c>
+      <c r="N10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1205</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1205</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1206</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1207</v>
+      </c>
+      <c r="G11" t="s">
+        <v>1205</v>
+      </c>
+      <c r="I11" t="s">
+        <v>1208</v>
+      </c>
+      <c r="J11" t="s">
+        <v>1209</v>
+      </c>
+      <c r="K11" t="s">
+        <v>1210</v>
+      </c>
+      <c r="L11" t="s">
+        <v>1211</v>
+      </c>
+      <c r="M11" t="s">
+        <v>1212</v>
+      </c>
+      <c r="N11" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1215</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1216</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1217</v>
+      </c>
+      <c r="G12" t="s">
+        <v>1215</v>
+      </c>
+      <c r="I12" t="s">
+        <v>796</v>
+      </c>
+      <c r="J12" t="s">
+        <v>1218</v>
+      </c>
+      <c r="K12" t="s">
+        <v>1218</v>
+      </c>
+      <c r="L12" t="s">
+        <v>1219</v>
+      </c>
+      <c r="M12" t="s">
+        <v>1220</v>
+      </c>
+      <c r="N12" t="s">
+        <v>1218</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="5" customFormat="1">
+      <c r="A13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>1221</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>1222</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>1223</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>1224</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>1225</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>1226</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>733</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>1227</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>1228</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>332</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>1229</v>
+      </c>
+      <c r="N13" s="5" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1232</v>
+      </c>
+      <c r="D14" t="s">
+        <v>817</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1233</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1234</v>
+      </c>
+      <c r="G14" t="s">
+        <v>1235</v>
+      </c>
+      <c r="I14" t="s">
+        <v>38</v>
+      </c>
+      <c r="J14" t="s">
+        <v>66</v>
+      </c>
+      <c r="K14" t="s">
+        <v>51</v>
+      </c>
+      <c r="L14" t="s">
+        <v>1236</v>
+      </c>
+      <c r="M14" t="s">
+        <v>73</v>
+      </c>
+      <c r="N14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC63772D-A536-435C-9164-B38BADB6850E}">
   <dimension ref="A1:N14"/>
   <sheetViews>
@@ -5625,12 +6182,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CECA0EB1-A2B3-4508-8794-059653B4E84D}">
   <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection sqref="A1:N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5793,7 +6350,421 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3295008-3AAD-4E89-BA77-04BE8FBA0B66}">
+  <dimension ref="A1:N14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:N14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49C139A8-B3CB-410B-ABD8-5A2BB2548BB4}">
+  <dimension ref="A1:N14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:N14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A0953B5-619C-4EFA-A4D9-2FCC751D70A8}">
+  <dimension ref="A1:N14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:N14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{938527A0-21F1-4AFC-8C1C-AAA3BBFAE52C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95533A0B-9A01-441D-8039-E1ACBF46589A}">
   <dimension ref="A1:N21"/>
   <sheetViews>
@@ -6375,7 +7346,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CFBAAD1-4C6B-447A-A9EB-0C496CC6460C}">
   <dimension ref="A1:N14"/>
   <sheetViews>
@@ -6928,7 +7899,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{452EE730-30E6-41DD-A76D-601E9AD8390E}">
   <dimension ref="A1:N14"/>
   <sheetViews>
@@ -7481,7 +8452,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E4A539E-735E-49C7-9BD4-7FFC27BC6B52}">
   <dimension ref="A1:N14"/>
   <sheetViews>
@@ -8043,7 +9014,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E9B1421-F51A-41E3-BAC4-EB64367C4DFF}">
   <dimension ref="A1:N14"/>
   <sheetViews>
@@ -8601,7 +9572,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3CA3735-64F7-4AF9-AFE5-A2AEC5283FC2}">
   <dimension ref="A1:N14"/>
   <sheetViews>
@@ -9154,7 +10125,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE42329A-79F3-4AE4-BC9A-7B3E54685DCD}">
   <dimension ref="A1:N14"/>
   <sheetViews>
@@ -9705,557 +10676,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E672E80F-B107-465D-99B6-B0D1191F61A9}">
-  <dimension ref="A1:N14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:14">
-      <c r="A1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" s="7" customFormat="1">
-      <c r="A3" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>1126</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>1127</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>1128</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>1129</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>1130</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>1131</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>1132</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>1133</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>1134</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>1135</v>
-      </c>
-      <c r="N3" s="7" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>873</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1136</v>
-      </c>
-      <c r="D4" t="s">
-        <v>1137</v>
-      </c>
-      <c r="E4" t="s">
-        <v>1138</v>
-      </c>
-      <c r="F4" t="s">
-        <v>1139</v>
-      </c>
-      <c r="G4" t="s">
-        <v>1140</v>
-      </c>
-      <c r="I4" t="s">
-        <v>1141</v>
-      </c>
-      <c r="J4" t="s">
-        <v>1142</v>
-      </c>
-      <c r="K4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L4" t="s">
-        <v>1143</v>
-      </c>
-      <c r="M4" t="s">
-        <v>1144</v>
-      </c>
-      <c r="N4" t="s">
-        <v>1145</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1146</v>
-      </c>
-      <c r="C5" t="s">
-        <v>1147</v>
-      </c>
-      <c r="D5" t="s">
-        <v>1148</v>
-      </c>
-      <c r="E5" t="s">
-        <v>1149</v>
-      </c>
-      <c r="F5" t="s">
-        <v>1150</v>
-      </c>
-      <c r="G5" t="s">
-        <v>1151</v>
-      </c>
-      <c r="I5" t="s">
-        <v>65</v>
-      </c>
-      <c r="J5" t="s">
-        <v>85</v>
-      </c>
-      <c r="K5" t="s">
-        <v>1152</v>
-      </c>
-      <c r="L5" t="s">
-        <v>1153</v>
-      </c>
-      <c r="M5" t="s">
-        <v>1154</v>
-      </c>
-      <c r="N5" t="s">
-        <v>1155</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1156</v>
-      </c>
-      <c r="C6" t="s">
-        <v>1157</v>
-      </c>
-      <c r="D6" t="s">
-        <v>1158</v>
-      </c>
-      <c r="E6" t="s">
-        <v>1159</v>
-      </c>
-      <c r="F6" t="s">
-        <v>148</v>
-      </c>
-      <c r="G6" t="s">
-        <v>1160</v>
-      </c>
-      <c r="I6" t="s">
-        <v>444</v>
-      </c>
-      <c r="J6" t="s">
-        <v>1161</v>
-      </c>
-      <c r="K6" t="s">
-        <v>1162</v>
-      </c>
-      <c r="L6" t="s">
-        <v>1163</v>
-      </c>
-      <c r="M6" t="s">
-        <v>1164</v>
-      </c>
-      <c r="N6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
-      <c r="A7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1165</v>
-      </c>
-      <c r="C7" t="s">
-        <v>1166</v>
-      </c>
-      <c r="D7" t="s">
-        <v>551</v>
-      </c>
-      <c r="E7" t="s">
-        <v>1167</v>
-      </c>
-      <c r="F7" t="s">
-        <v>1168</v>
-      </c>
-      <c r="G7" t="s">
-        <v>1169</v>
-      </c>
-      <c r="I7" t="s">
-        <v>925</v>
-      </c>
-      <c r="J7" t="s">
-        <v>1170</v>
-      </c>
-      <c r="K7" t="s">
-        <v>1171</v>
-      </c>
-      <c r="L7" t="s">
-        <v>1172</v>
-      </c>
-      <c r="M7" t="s">
-        <v>78</v>
-      </c>
-      <c r="N7" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" s="5" customFormat="1">
-      <c r="A8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>1173</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>1174</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>1175</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>1176</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>1177</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>1178</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>1179</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>1180</v>
-      </c>
-      <c r="L8" s="5" t="s">
-        <v>1181</v>
-      </c>
-      <c r="M8" s="5" t="s">
-        <v>1182</v>
-      </c>
-      <c r="N8" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
-      <c r="A9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1183</v>
-      </c>
-      <c r="C9" t="s">
-        <v>1184</v>
-      </c>
-      <c r="D9" t="s">
-        <v>1185</v>
-      </c>
-      <c r="E9" t="s">
-        <v>1186</v>
-      </c>
-      <c r="F9" t="s">
-        <v>628</v>
-      </c>
-      <c r="G9" t="s">
-        <v>1187</v>
-      </c>
-      <c r="I9" t="s">
-        <v>1188</v>
-      </c>
-      <c r="J9" t="s">
-        <v>1189</v>
-      </c>
-      <c r="K9" t="s">
-        <v>1190</v>
-      </c>
-      <c r="L9" t="s">
-        <v>1191</v>
-      </c>
-      <c r="M9" t="s">
-        <v>1192</v>
-      </c>
-      <c r="N9" t="s">
-        <v>1193</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="A10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1194</v>
-      </c>
-      <c r="C10" t="s">
-        <v>1195</v>
-      </c>
-      <c r="D10" t="s">
-        <v>1196</v>
-      </c>
-      <c r="E10" t="s">
-        <v>1197</v>
-      </c>
-      <c r="F10" t="s">
-        <v>1198</v>
-      </c>
-      <c r="G10" t="s">
-        <v>1199</v>
-      </c>
-      <c r="I10" t="s">
-        <v>1200</v>
-      </c>
-      <c r="J10" t="s">
-        <v>41</v>
-      </c>
-      <c r="K10" t="s">
-        <v>1201</v>
-      </c>
-      <c r="L10" t="s">
-        <v>1202</v>
-      </c>
-      <c r="M10" t="s">
-        <v>1203</v>
-      </c>
-      <c r="N10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="A11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1204</v>
-      </c>
-      <c r="C11" t="s">
-        <v>1205</v>
-      </c>
-      <c r="D11" t="s">
-        <v>1205</v>
-      </c>
-      <c r="E11" t="s">
-        <v>1206</v>
-      </c>
-      <c r="F11" t="s">
-        <v>1207</v>
-      </c>
-      <c r="G11" t="s">
-        <v>1205</v>
-      </c>
-      <c r="I11" t="s">
-        <v>1208</v>
-      </c>
-      <c r="J11" t="s">
-        <v>1209</v>
-      </c>
-      <c r="K11" t="s">
-        <v>1210</v>
-      </c>
-      <c r="L11" t="s">
-        <v>1211</v>
-      </c>
-      <c r="M11" t="s">
-        <v>1212</v>
-      </c>
-      <c r="N11" t="s">
-        <v>1213</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
-      <c r="A12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s">
-        <v>1214</v>
-      </c>
-      <c r="C12" t="s">
-        <v>1215</v>
-      </c>
-      <c r="D12" t="s">
-        <v>1215</v>
-      </c>
-      <c r="E12" t="s">
-        <v>1216</v>
-      </c>
-      <c r="F12" t="s">
-        <v>1217</v>
-      </c>
-      <c r="G12" t="s">
-        <v>1215</v>
-      </c>
-      <c r="I12" t="s">
-        <v>796</v>
-      </c>
-      <c r="J12" t="s">
-        <v>1218</v>
-      </c>
-      <c r="K12" t="s">
-        <v>1218</v>
-      </c>
-      <c r="L12" t="s">
-        <v>1219</v>
-      </c>
-      <c r="M12" t="s">
-        <v>1220</v>
-      </c>
-      <c r="N12" t="s">
-        <v>1218</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" s="5" customFormat="1">
-      <c r="A13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>1221</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>1222</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>1223</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>1224</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>1225</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>1226</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>733</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>1227</v>
-      </c>
-      <c r="K13" s="5" t="s">
-        <v>1228</v>
-      </c>
-      <c r="L13" s="5" t="s">
-        <v>332</v>
-      </c>
-      <c r="M13" s="5" t="s">
-        <v>1229</v>
-      </c>
-      <c r="N13" s="5" t="s">
-        <v>1230</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
-      <c r="A14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" t="s">
-        <v>1231</v>
-      </c>
-      <c r="C14" t="s">
-        <v>1232</v>
-      </c>
-      <c r="D14" t="s">
-        <v>817</v>
-      </c>
-      <c r="E14" t="s">
-        <v>1233</v>
-      </c>
-      <c r="F14" t="s">
-        <v>1234</v>
-      </c>
-      <c r="G14" t="s">
-        <v>1235</v>
-      </c>
-      <c r="I14" t="s">
-        <v>38</v>
-      </c>
-      <c r="J14" t="s">
-        <v>66</v>
-      </c>
-      <c r="K14" t="s">
-        <v>51</v>
-      </c>
-      <c r="L14" t="s">
-        <v>1236</v>
-      </c>
-      <c r="M14" t="s">
-        <v>73</v>
-      </c>
-      <c r="N14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
added postag result for TT.
</commit_message>
<xml_diff>
--- a/output/TTTT.xlsx
+++ b/output/TTTT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pree\Thai_SA_journal\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E223C03D-CFD3-4A6D-90EE-024811127DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05AB4484-B6A7-4CE0-AC45-BE20371469D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="5" activeTab="14" xr2:uid="{9BDD03C8-F7C5-4674-9603-EB57B3FD651B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="5" activeTab="12" xr2:uid="{9BDD03C8-F7C5-4674-9603-EB57B3FD651B}"/>
   </bookViews>
   <sheets>
     <sheet name="BOW1" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1804" uniqueCount="1354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2380" uniqueCount="1795">
   <si>
     <t>SVM</t>
   </si>
@@ -4111,6 +4111,1329 @@
   </si>
   <si>
     <t>0.432±0.434</t>
+  </si>
+  <si>
+    <t>0.4784±0.0</t>
+  </si>
+  <si>
+    <t>0.1595±0.0</t>
+  </si>
+  <si>
+    <t>0.3333±0.0</t>
+  </si>
+  <si>
+    <t>0.0±0.0</t>
+  </si>
+  <si>
+    <t>0.5±0.0</t>
+  </si>
+  <si>
+    <t>0.2157±0.0</t>
+  </si>
+  <si>
+    <t>0.329±0.1062</t>
+  </si>
+  <si>
+    <t>0.1097±0.0354</t>
+  </si>
+  <si>
+    <t>0.1623±0.0384</t>
+  </si>
+  <si>
+    <t>0.5099±0.0108</t>
+  </si>
+  <si>
+    <t>0.4959±0.0539</t>
+  </si>
+  <si>
+    <t>0.3905±0.0174</t>
+  </si>
+  <si>
+    <t>0.1541±0.0276</t>
+  </si>
+  <si>
+    <t>0.6139±0.0118</t>
+  </si>
+  <si>
+    <t>0.4354±0.0233</t>
+  </si>
+  <si>
+    <t>0.5003±0.0137</t>
+  </si>
+  <si>
+    <t>0.4789±0.0663</t>
+  </si>
+  <si>
+    <t>0.3845±0.0186</t>
+  </si>
+  <si>
+    <t>0.1316±0.0346</t>
+  </si>
+  <si>
+    <t>0.6105±0.0219</t>
+  </si>
+  <si>
+    <t>0.4247±0.0312</t>
+  </si>
+  <si>
+    <t>0.5099±0.0074</t>
+  </si>
+  <si>
+    <t>0.5988±0.1009</t>
+  </si>
+  <si>
+    <t>0.3784±0.0134</t>
+  </si>
+  <si>
+    <t>0.1577±0.0207</t>
+  </si>
+  <si>
+    <t>0.6119±0.0224</t>
+  </si>
+  <si>
+    <t>0.4607±0.0332</t>
+  </si>
+  <si>
+    <t>0.5127±0.013</t>
+  </si>
+  <si>
+    <t>0.5104±0.0197</t>
+  </si>
+  <si>
+    <t>0.3938±0.0156</t>
+  </si>
+  <si>
+    <t>0.1577±0.033</t>
+  </si>
+  <si>
+    <t>0.6122±0.0211</t>
+  </si>
+  <si>
+    <t>0.4445±0.0169</t>
+  </si>
+  <si>
+    <t>0.5074±0.0091</t>
+  </si>
+  <si>
+    <t>0.5402±0.111</t>
+  </si>
+  <si>
+    <t>0.3766±0.0151</t>
+  </si>
+  <si>
+    <t>0.1462±0.0257</t>
+  </si>
+  <si>
+    <t>0.6129±0.0164</t>
+  </si>
+  <si>
+    <t>0.4398±0.0453</t>
+  </si>
+  <si>
+    <t>0.5109±0.0102</t>
+  </si>
+  <si>
+    <t>0.5851±0.1073</t>
+  </si>
+  <si>
+    <t>0.3856±0.0156</t>
+  </si>
+  <si>
+    <t>0.1584±0.0276</t>
+  </si>
+  <si>
+    <t>0.6124±0.0151</t>
+  </si>
+  <si>
+    <t>0.4604±0.0336</t>
+  </si>
+  <si>
+    <t>0.4931±0.0127</t>
+  </si>
+  <si>
+    <t>0.4752±0.0368</t>
+  </si>
+  <si>
+    <t>0.4099±0.0216</t>
+  </si>
+  <si>
+    <t>0.1387±0.0336</t>
+  </si>
+  <si>
+    <t>0.6044±0.009</t>
+  </si>
+  <si>
+    <t>0.4395±0.0218</t>
+  </si>
+  <si>
+    <t>0.4911±0.0173</t>
+  </si>
+  <si>
+    <t>0.4658±0.071</t>
+  </si>
+  <si>
+    <t>0.3754±0.0146</t>
+  </si>
+  <si>
+    <t>0.1058±0.0421</t>
+  </si>
+  <si>
+    <t>0.6134±0.02</t>
+  </si>
+  <si>
+    <t>0.4141±0.0335</t>
+  </si>
+  <si>
+    <t>0.4644±0.0184</t>
+  </si>
+  <si>
+    <t>0.3799±0.0314</t>
+  </si>
+  <si>
+    <t>0.3529±0.0134</t>
+  </si>
+  <si>
+    <t>0.0487±0.0368</t>
+  </si>
+  <si>
+    <t>0.5147±0.0101</t>
+  </si>
+  <si>
+    <t>0.3657±0.0214</t>
+  </si>
+  <si>
+    <t>0.4733±0.0275</t>
+  </si>
+  <si>
+    <t>0.4057±0.0526</t>
+  </si>
+  <si>
+    <t>0.3774±0.0212</t>
+  </si>
+  <si>
+    <t>0.094±0.0411</t>
+  </si>
+  <si>
+    <t>0.533±0.0159</t>
+  </si>
+  <si>
+    <t>0.3902±0.0349</t>
+  </si>
+  <si>
+    <t>0.5031±0.0124</t>
+  </si>
+  <si>
+    <t>0.4918±0.1581</t>
+  </si>
+  <si>
+    <t>0.3728±0.0194</t>
+  </si>
+  <si>
+    <t>0.1314±0.053</t>
+  </si>
+  <si>
+    <t>0.6173±0.0166</t>
+  </si>
+  <si>
+    <t>0.4136±0.0764</t>
+  </si>
+  <si>
+    <t>0.5074±0.0132</t>
+  </si>
+  <si>
+    <t>0.5095±0.0601</t>
+  </si>
+  <si>
+    <t>0.3892±0.0141</t>
+  </si>
+  <si>
+    <t>0.1454±0.0347</t>
+  </si>
+  <si>
+    <t>0.6289±0.0192</t>
+  </si>
+  <si>
+    <t>0.4401±0.0282</t>
+  </si>
+  <si>
+    <t>0.5041±0.0127</t>
+  </si>
+  <si>
+    <t>0.4743±0.0418</t>
+  </si>
+  <si>
+    <t>0.3972±0.0172</t>
+  </si>
+  <si>
+    <t>0.1482±0.0304</t>
+  </si>
+  <si>
+    <t>0.6195±0.0234</t>
+  </si>
+  <si>
+    <t>0.4314±0.0191</t>
+  </si>
+  <si>
+    <t>0.4975±0.0229</t>
+  </si>
+  <si>
+    <t>0.4533±0.0314</t>
+  </si>
+  <si>
+    <t>0.4077±0.0184</t>
+  </si>
+  <si>
+    <t>0.1462±0.0397</t>
+  </si>
+  <si>
+    <t>0.6052±0.0194</t>
+  </si>
+  <si>
+    <t>0.4292±0.0237</t>
+  </si>
+  <si>
+    <t>0.4506±0.0324</t>
+  </si>
+  <si>
+    <t>0.4035±0.0411</t>
+  </si>
+  <si>
+    <t>0.3952±0.0363</t>
+  </si>
+  <si>
+    <t>0.0994±0.0568</t>
+  </si>
+  <si>
+    <t>0.589±0.0309</t>
+  </si>
+  <si>
+    <t>0.3993±0.0386</t>
+  </si>
+  <si>
+    <t>0.4321±0.026</t>
+  </si>
+  <si>
+    <t>0.3908±0.0325</t>
+  </si>
+  <si>
+    <t>0.3879±0.0296</t>
+  </si>
+  <si>
+    <t>0.0852±0.0444</t>
+  </si>
+  <si>
+    <t>0.5802±0.026</t>
+  </si>
+  <si>
+    <t>0.3893±0.031</t>
+  </si>
+  <si>
+    <t>0.4929±0.0114</t>
+  </si>
+  <si>
+    <t>0.4419±0.0258</t>
+  </si>
+  <si>
+    <t>0.4042±0.015</t>
+  </si>
+  <si>
+    <t>0.1371±0.0238</t>
+  </si>
+  <si>
+    <t>0.6138±0.0217</t>
+  </si>
+  <si>
+    <t>0.4221±0.0195</t>
+  </si>
+  <si>
+    <t>0.4743±0.0199</t>
+  </si>
+  <si>
+    <t>0.4332±0.0291</t>
+  </si>
+  <si>
+    <t>0.4223±0.0261</t>
+  </si>
+  <si>
+    <t>0.1422±0.0362</t>
+  </si>
+  <si>
+    <t>0.6037±0.0274</t>
+  </si>
+  <si>
+    <t>0.4277±0.0274</t>
+  </si>
+  <si>
+    <t>0.4481±0.0184</t>
+  </si>
+  <si>
+    <t>0.4083±0.0189</t>
+  </si>
+  <si>
+    <t>0.4049±0.018</t>
+  </si>
+  <si>
+    <t>0.1122±0.0287</t>
+  </si>
+  <si>
+    <t>0.5701±0.0168</t>
+  </si>
+  <si>
+    <t>0.4066±0.0184</t>
+  </si>
+  <si>
+    <t>0.4919±0.0114</t>
+  </si>
+  <si>
+    <t>0.4344±0.0403</t>
+  </si>
+  <si>
+    <t>0.3703±0.0103</t>
+  </si>
+  <si>
+    <t>0.1033±0.0282</t>
+  </si>
+  <si>
+    <t>0.5989±0.0169</t>
+  </si>
+  <si>
+    <t>0.3993±0.0219</t>
+  </si>
+  <si>
+    <t>0.4234±0.0287</t>
+  </si>
+  <si>
+    <t>0.3797±0.0239</t>
+  </si>
+  <si>
+    <t>0.3769±0.0225</t>
+  </si>
+  <si>
+    <t>0.0736±0.0367</t>
+  </si>
+  <si>
+    <t>0.5327±0.0169</t>
+  </si>
+  <si>
+    <t>0.3783±0.0232</t>
+  </si>
+  <si>
+    <t>0.4112±0.031</t>
+  </si>
+  <si>
+    <t>0.3854±0.0274</t>
+  </si>
+  <si>
+    <t>0.3844±0.0257</t>
+  </si>
+  <si>
+    <t>0.0802±0.0397</t>
+  </si>
+  <si>
+    <t>0.5348±0.0186</t>
+  </si>
+  <si>
+    <t>0.3849±0.0265</t>
+  </si>
+  <si>
+    <t>0.5046±0.0201</t>
+  </si>
+  <si>
+    <t>0.4605±0.1197</t>
+  </si>
+  <si>
+    <t>0.3939±0.0312</t>
+  </si>
+  <si>
+    <t>0.1379±0.0615</t>
+  </si>
+  <si>
+    <t>0.6251±0.0197</t>
+  </si>
+  <si>
+    <t>0.4183±0.0759</t>
+  </si>
+  <si>
+    <t>0.5056±0.015</t>
+  </si>
+  <si>
+    <t>0.4742±0.0375</t>
+  </si>
+  <si>
+    <t>0.4027±0.0144</t>
+  </si>
+  <si>
+    <t>0.1494±0.0304</t>
+  </si>
+  <si>
+    <t>0.6337±0.0172</t>
+  </si>
+  <si>
+    <t>0.4353±0.0235</t>
+  </si>
+  <si>
+    <t>0.5313±0.0159</t>
+  </si>
+  <si>
+    <t>0.5127±0.0286</t>
+  </si>
+  <si>
+    <t>0.4283±0.0244</t>
+  </si>
+  <si>
+    <t>0.2054±0.0339</t>
+  </si>
+  <si>
+    <t>0.6407±0.018</t>
+  </si>
+  <si>
+    <t>0.4664±0.0226</t>
+  </si>
+  <si>
+    <t>0.5219±0.019</t>
+  </si>
+  <si>
+    <t>0.501±0.0374</t>
+  </si>
+  <si>
+    <t>0.4117±0.0209</t>
+  </si>
+  <si>
+    <t>0.1833±0.0425</t>
+  </si>
+  <si>
+    <t>0.6289±0.0325</t>
+  </si>
+  <si>
+    <t>0.4515±0.0228</t>
+  </si>
+  <si>
+    <t>0.528±0.0137</t>
+  </si>
+  <si>
+    <t>0.5495±0.0418</t>
+  </si>
+  <si>
+    <t>0.4111±0.0227</t>
+  </si>
+  <si>
+    <t>0.1978±0.0349</t>
+  </si>
+  <si>
+    <t>0.6482±0.0248</t>
+  </si>
+  <si>
+    <t>0.4694±0.0214</t>
+  </si>
+  <si>
+    <t>0.5336±0.0249</t>
+  </si>
+  <si>
+    <t>0.5064±0.0423</t>
+  </si>
+  <si>
+    <t>0.4367±0.0301</t>
+  </si>
+  <si>
+    <t>0.2108±0.0554</t>
+  </si>
+  <si>
+    <t>0.6495±0.0241</t>
+  </si>
+  <si>
+    <t>0.4688±0.0336</t>
+  </si>
+  <si>
+    <t>0.5333±0.0219</t>
+  </si>
+  <si>
+    <t>0.53±0.0564</t>
+  </si>
+  <si>
+    <t>0.4235±0.0328</t>
+  </si>
+  <si>
+    <t>0.2087±0.0497</t>
+  </si>
+  <si>
+    <t>0.6419±0.0297</t>
+  </si>
+  <si>
+    <t>0.4698±0.036</t>
+  </si>
+  <si>
+    <t>0.5318±0.0126</t>
+  </si>
+  <si>
+    <t>0.5717±0.0514</t>
+  </si>
+  <si>
+    <t>0.4126±0.016</t>
+  </si>
+  <si>
+    <t>0.207±0.0302</t>
+  </si>
+  <si>
+    <t>0.6573±0.0247</t>
+  </si>
+  <si>
+    <t>0.4786±0.0255</t>
+  </si>
+  <si>
+    <t>0.5328±0.0138</t>
+  </si>
+  <si>
+    <t>0.5236±0.0219</t>
+  </si>
+  <si>
+    <t>0.4325±0.0151</t>
+  </si>
+  <si>
+    <t>0.2101±0.0287</t>
+  </si>
+  <si>
+    <t>0.6187±0.0224</t>
+  </si>
+  <si>
+    <t>0.4735±0.0148</t>
+  </si>
+  <si>
+    <t>0.5298±0.028</t>
+  </si>
+  <si>
+    <t>0.4992±0.0553</t>
+  </si>
+  <si>
+    <t>0.4335±0.0274</t>
+  </si>
+  <si>
+    <t>0.2053±0.054</t>
+  </si>
+  <si>
+    <t>0.6481±0.0219</t>
+  </si>
+  <si>
+    <t>0.4637±0.0393</t>
+  </si>
+  <si>
+    <t>0.4438±0.0197</t>
+  </si>
+  <si>
+    <t>0.3845±0.0271</t>
+  </si>
+  <si>
+    <t>0.3824±0.0246</t>
+  </si>
+  <si>
+    <t>0.0871±0.0393</t>
+  </si>
+  <si>
+    <t>0.5368±0.0185</t>
+  </si>
+  <si>
+    <t>0.3834±0.0257</t>
+  </si>
+  <si>
+    <t>0.4099±0.0645</t>
+  </si>
+  <si>
+    <t>0.3837±0.0337</t>
+  </si>
+  <si>
+    <t>0.3876±0.0348</t>
+  </si>
+  <si>
+    <t>0.0905±0.0527</t>
+  </si>
+  <si>
+    <t>0.5407±0.0261</t>
+  </si>
+  <si>
+    <t>0.3856±0.0338</t>
+  </si>
+  <si>
+    <t>0.5239±0.0221</t>
+  </si>
+  <si>
+    <t>0.5452±0.0627</t>
+  </si>
+  <si>
+    <t>0.4021±0.0305</t>
+  </si>
+  <si>
+    <t>0.186±0.0513</t>
+  </si>
+  <si>
+    <t>0.6428±0.0192</t>
+  </si>
+  <si>
+    <t>0.4618±0.0382</t>
+  </si>
+  <si>
+    <t>0.5336±0.0196</t>
+  </si>
+  <si>
+    <t>0.5331±0.0454</t>
+  </si>
+  <si>
+    <t>0.4246±0.0196</t>
+  </si>
+  <si>
+    <t>0.2091±0.0429</t>
+  </si>
+  <si>
+    <t>0.6704±0.0214</t>
+  </si>
+  <si>
+    <t>0.4723±0.0283</t>
+  </si>
+  <si>
+    <t>0.5084±0.024</t>
+  </si>
+  <si>
+    <t>0.4665±0.0255</t>
+  </si>
+  <si>
+    <t>0.4374±0.0263</t>
+  </si>
+  <si>
+    <t>0.1876±0.0334</t>
+  </si>
+  <si>
+    <t>0.6501±0.0245</t>
+  </si>
+  <si>
+    <t>0.4512±0.0231</t>
+  </si>
+  <si>
+    <t>0.5224±0.0278</t>
+  </si>
+  <si>
+    <t>0.4807±0.0345</t>
+  </si>
+  <si>
+    <t>0.4552±0.024</t>
+  </si>
+  <si>
+    <t>0.2122±0.0444</t>
+  </si>
+  <si>
+    <t>0.6457±0.022</t>
+  </si>
+  <si>
+    <t>0.4675±0.0288</t>
+  </si>
+  <si>
+    <t>0.5232±0.0234</t>
+  </si>
+  <si>
+    <t>0.4773±0.0308</t>
+  </si>
+  <si>
+    <t>0.4447±0.0221</t>
+  </si>
+  <si>
+    <t>0.205±0.04</t>
+  </si>
+  <si>
+    <t>0.6508±0.0185</t>
+  </si>
+  <si>
+    <t>0.4603±0.0256</t>
+  </si>
+  <si>
+    <t>0.5102±0.0339</t>
+  </si>
+  <si>
+    <t>0.4605±0.0447</t>
+  </si>
+  <si>
+    <t>0.4415±0.0319</t>
+  </si>
+  <si>
+    <t>0.1913±0.0551</t>
+  </si>
+  <si>
+    <t>0.6423±0.0239</t>
+  </si>
+  <si>
+    <t>0.4507±0.0379</t>
+  </si>
+  <si>
+    <t>0.5196±0.0302</t>
+  </si>
+  <si>
+    <t>0.4749±0.0433</t>
+  </si>
+  <si>
+    <t>0.4528±0.0306</t>
+  </si>
+  <si>
+    <t>0.2083±0.0508</t>
+  </si>
+  <si>
+    <t>0.6522±0.0231</t>
+  </si>
+  <si>
+    <t>0.4635±0.0363</t>
+  </si>
+  <si>
+    <t>0.5117±0.029</t>
+  </si>
+  <si>
+    <t>0.4735±0.0385</t>
+  </si>
+  <si>
+    <t>0.4609±0.0319</t>
+  </si>
+  <si>
+    <t>0.2068±0.0477</t>
+  </si>
+  <si>
+    <t>0.6494±0.0259</t>
+  </si>
+  <si>
+    <t>0.4671±0.0349</t>
+  </si>
+  <si>
+    <t>0.4969±0.0222</t>
+  </si>
+  <si>
+    <t>0.4587±0.025</t>
+  </si>
+  <si>
+    <t>0.4471±0.0207</t>
+  </si>
+  <si>
+    <t>0.1845±0.0343</t>
+  </si>
+  <si>
+    <t>0.6237±0.0216</t>
+  </si>
+  <si>
+    <t>0.4528±0.0224</t>
+  </si>
+  <si>
+    <t>0.5272±0.0126</t>
+  </si>
+  <si>
+    <t>0.4905±0.019</t>
+  </si>
+  <si>
+    <t>0.4294±0.0115</t>
+  </si>
+  <si>
+    <t>0.199±0.0251</t>
+  </si>
+  <si>
+    <t>0.6371±0.018</t>
+  </si>
+  <si>
+    <t>0.4579±0.0146</t>
+  </si>
+  <si>
+    <t>0.4313±0.0351</t>
+  </si>
+  <si>
+    <t>0.3769±0.0394</t>
+  </si>
+  <si>
+    <t>0.3739±0.0328</t>
+  </si>
+  <si>
+    <t>0.0731±0.0529</t>
+  </si>
+  <si>
+    <t>0.5305±0.0246</t>
+  </si>
+  <si>
+    <t>0.3754±0.036</t>
+  </si>
+  <si>
+    <t>0.4425±0.0249</t>
+  </si>
+  <si>
+    <t>0.4057±0.0234</t>
+  </si>
+  <si>
+    <t>0.4047±0.0224</t>
+  </si>
+  <si>
+    <t>0.1198±0.0339</t>
+  </si>
+  <si>
+    <t>0.5526±0.016</t>
+  </si>
+  <si>
+    <t>0.4052±0.0229</t>
+  </si>
+  <si>
+    <t>0.527±0.0304</t>
+  </si>
+  <si>
+    <t>0.4888±0.0421</t>
+  </si>
+  <si>
+    <t>0.4416±0.0355</t>
+  </si>
+  <si>
+    <t>0.2088±0.0537</t>
+  </si>
+  <si>
+    <t>0.6628±0.0218</t>
+  </si>
+  <si>
+    <t>0.4635±0.0355</t>
+  </si>
+  <si>
+    <t>0.542±0.0211</t>
+  </si>
+  <si>
+    <t>0.5121±0.0338</t>
+  </si>
+  <si>
+    <t>0.4568±0.0213</t>
+  </si>
+  <si>
+    <t>0.2332±0.0393</t>
+  </si>
+  <si>
+    <t>0.669±0.0193</t>
+  </si>
+  <si>
+    <t>0.4828±0.0267</t>
+  </si>
+  <si>
+    <t>0.5112±0.0108</t>
+  </si>
+  <si>
+    <t>0.4654±0.0568</t>
+  </si>
+  <si>
+    <t>0.3957±0.0107</t>
+  </si>
+  <si>
+    <t>0.1576±0.0219</t>
+  </si>
+  <si>
+    <t>0.5943±0.0125</t>
+  </si>
+  <si>
+    <t>0.4264±0.0251</t>
+  </si>
+  <si>
+    <t>0.4997±0.0088</t>
+  </si>
+  <si>
+    <t>0.4533±0.1051</t>
+  </si>
+  <si>
+    <t>0.3773±0.0132</t>
+  </si>
+  <si>
+    <t>0.1225±0.0258</t>
+  </si>
+  <si>
+    <t>0.591±0.0181</t>
+  </si>
+  <si>
+    <t>0.4074±0.0454</t>
+  </si>
+  <si>
+    <t>0.4809±0.0236</t>
+  </si>
+  <si>
+    <t>0.4141±0.0357</t>
+  </si>
+  <si>
+    <t>0.4001±0.0219</t>
+  </si>
+  <si>
+    <t>0.1282±0.0392</t>
+  </si>
+  <si>
+    <t>0.5832±0.0143</t>
+  </si>
+  <si>
+    <t>0.4068±0.0281</t>
+  </si>
+  <si>
+    <t>0.474±0.0206</t>
+  </si>
+  <si>
+    <t>0.4051±0.0278</t>
+  </si>
+  <si>
+    <t>0.3949±0.0166</t>
+  </si>
+  <si>
+    <t>0.1181±0.0318</t>
+  </si>
+  <si>
+    <t>0.5808±0.0148</t>
+  </si>
+  <si>
+    <t>0.3998±0.0218</t>
+  </si>
+  <si>
+    <t>0.4969±0.0195</t>
+  </si>
+  <si>
+    <t>0.4319±0.0175</t>
+  </si>
+  <si>
+    <t>0.4151±0.014</t>
+  </si>
+  <si>
+    <t>0.158±0.0318</t>
+  </si>
+  <si>
+    <t>0.5892±0.0146</t>
+  </si>
+  <si>
+    <t>0.4233±0.0153</t>
+  </si>
+  <si>
+    <t>0.4896±0.027</t>
+  </si>
+  <si>
+    <t>0.4291±0.0364</t>
+  </si>
+  <si>
+    <t>0.4085±0.0231</t>
+  </si>
+  <si>
+    <t>0.1434±0.0448</t>
+  </si>
+  <si>
+    <t>0.5861±0.0195</t>
+  </si>
+  <si>
+    <t>0.4184±0.0294</t>
+  </si>
+  <si>
+    <t>0.486±0.0194</t>
+  </si>
+  <si>
+    <t>0.423±0.0273</t>
+  </si>
+  <si>
+    <t>0.4107±0.0213</t>
+  </si>
+  <si>
+    <t>0.144±0.0345</t>
+  </si>
+  <si>
+    <t>0.5943±0.008</t>
+  </si>
+  <si>
+    <t>0.4167±0.024</t>
+  </si>
+  <si>
+    <t>0.4804±0.0052</t>
+  </si>
+  <si>
+    <t>0.265±0.085</t>
+  </si>
+  <si>
+    <t>0.3368±0.0062</t>
+  </si>
+  <si>
+    <t>0.0262±0.0377</t>
+  </si>
+  <si>
+    <t>0.59±0.014</t>
+  </si>
+  <si>
+    <t>0.2902±0.0576</t>
+  </si>
+  <si>
+    <t>0.3812±0.0238</t>
+  </si>
+  <si>
+    <t>0.3463±0.0242</t>
+  </si>
+  <si>
+    <t>0.346±0.0246</t>
+  </si>
+  <si>
+    <t>0.0239±0.0371</t>
+  </si>
+  <si>
+    <t>0.5095±0.0185</t>
+  </si>
+  <si>
+    <t>0.3461±0.0244</t>
+  </si>
+  <si>
+    <t>0.4084±0.0258</t>
+  </si>
+  <si>
+    <t>0.3718±0.0198</t>
+  </si>
+  <si>
+    <t>0.3714±0.0192</t>
+  </si>
+  <si>
+    <t>0.0671±0.0323</t>
+  </si>
+  <si>
+    <t>0.5253±0.0153</t>
+  </si>
+  <si>
+    <t>0.3716±0.0195</t>
+  </si>
+  <si>
+    <t>0.5±0.0061</t>
+  </si>
+  <si>
+    <t>0.4599±0.1132</t>
+  </si>
+  <si>
+    <t>0.3782±0.0128</t>
+  </si>
+  <si>
+    <t>0.1282±0.0173</t>
+  </si>
+  <si>
+    <t>0.5931±0.0168</t>
+  </si>
+  <si>
+    <t>0.4098±0.0429</t>
+  </si>
+  <si>
+    <t>0.4936±0.0135</t>
+  </si>
+  <si>
+    <t>0.4262±0.0511</t>
+  </si>
+  <si>
+    <t>0.379±0.0115</t>
+  </si>
+  <si>
+    <t>0.1159±0.0292</t>
+  </si>
+  <si>
+    <t>0.5911±0.0143</t>
+  </si>
+  <si>
+    <t>0.4003±0.0278</t>
+  </si>
+  <si>
+    <t>0.4964±0.0204</t>
+  </si>
+  <si>
+    <t>0.4207±0.0544</t>
+  </si>
+  <si>
+    <t>0.3834±0.0107</t>
+  </si>
+  <si>
+    <t>0.1286±0.0387</t>
+  </si>
+  <si>
+    <t>0.5917±0.0194</t>
+  </si>
+  <si>
+    <t>0.4±0.0286</t>
+  </si>
+  <si>
+    <t>0.4863±0.0144</t>
+  </si>
+  <si>
+    <t>0.3916±0.0787</t>
+  </si>
+  <si>
+    <t>0.3662±0.0126</t>
+  </si>
+  <si>
+    <t>0.0907±0.0347</t>
+  </si>
+  <si>
+    <t>0.5881±0.0192</t>
+  </si>
+  <si>
+    <t>0.3756±0.0417</t>
+  </si>
+  <si>
+    <t>0.4667±0.0255</t>
+  </si>
+  <si>
+    <t>0.3877±0.0332</t>
+  </si>
+  <si>
+    <t>0.3827±0.0223</t>
+  </si>
+  <si>
+    <t>0.1018±0.0399</t>
+  </si>
+  <si>
+    <t>0.5763±0.0205</t>
+  </si>
+  <si>
+    <t>0.3851±0.0275</t>
+  </si>
+  <si>
+    <t>0.4697±0.0145</t>
+  </si>
+  <si>
+    <t>0.4003±0.021</t>
+  </si>
+  <si>
+    <t>0.3915±0.0159</t>
+  </si>
+  <si>
+    <t>0.112±0.0248</t>
+  </si>
+  <si>
+    <t>0.5766±0.0172</t>
+  </si>
+  <si>
+    <t>0.3959±0.0183</t>
+  </si>
+  <si>
+    <t>0.4504±0.0252</t>
+  </si>
+  <si>
+    <t>0.3823±0.027</t>
+  </si>
+  <si>
+    <t>0.3817±0.024</t>
+  </si>
+  <si>
+    <t>0.0928±0.0419</t>
+  </si>
+  <si>
+    <t>0.5623±0.0184</t>
+  </si>
+  <si>
+    <t>0.3819±0.0254</t>
+  </si>
+  <si>
+    <t>0.4369±0.0143</t>
+  </si>
+  <si>
+    <t>0.3695±0.0239</t>
+  </si>
+  <si>
+    <t>0.372±0.0177</t>
+  </si>
+  <si>
+    <t>0.0772±0.0255</t>
+  </si>
+  <si>
+    <t>0.5582±0.0165</t>
+  </si>
+  <si>
+    <t>0.3707±0.0207</t>
+  </si>
+  <si>
+    <t>0.4791±0.02</t>
+  </si>
+  <si>
+    <t>0.4126±0.0317</t>
+  </si>
+  <si>
+    <t>0.3976±0.0166</t>
+  </si>
+  <si>
+    <t>0.1248±0.0317</t>
+  </si>
+  <si>
+    <t>0.597±0.0153</t>
+  </si>
+  <si>
+    <t>0.4048±0.0233</t>
+  </si>
+  <si>
+    <t>0.4802±0.0036</t>
+  </si>
+  <si>
+    <t>0.3655±0.144</t>
+  </si>
+  <si>
+    <t>0.3363±0.0037</t>
+  </si>
+  <si>
+    <t>0.0326±0.0378</t>
+  </si>
+  <si>
+    <t>0.5901±0.0208</t>
+  </si>
+  <si>
+    <t>0.3393±0.0661</t>
+  </si>
+  <si>
+    <t>0.3916±0.0185</t>
+  </si>
+  <si>
+    <t>0.3584±0.0219</t>
+  </si>
+  <si>
+    <t>0.3586±0.0215</t>
+  </si>
+  <si>
+    <t>0.0395±0.0328</t>
+  </si>
+  <si>
+    <t>0.519±0.0161</t>
+  </si>
+  <si>
+    <t>0.3585±0.0217</t>
+  </si>
+  <si>
+    <t>0.415±0.0215</t>
+  </si>
+  <si>
+    <t>0.3792±0.0226</t>
+  </si>
+  <si>
+    <t>0.3789±0.0216</t>
+  </si>
+  <si>
+    <t>0.0748±0.0332</t>
+  </si>
+  <si>
+    <t>0.5302±0.0152</t>
+  </si>
+  <si>
+    <t>0.3791±0.0221</t>
+  </si>
+  <si>
+    <t>0.4906±0.0092</t>
+  </si>
+  <si>
+    <t>0.4085±0.069</t>
+  </si>
+  <si>
+    <t>0.3694±0.0163</t>
+  </si>
+  <si>
+    <t>0.0987±0.0327</t>
+  </si>
+  <si>
+    <t>0.5905±0.0216</t>
+  </si>
+  <si>
+    <t>0.3855±0.036</t>
+  </si>
+  <si>
+    <t>0.4908±0.0128</t>
+  </si>
+  <si>
+    <t>0.4285±0.0351</t>
+  </si>
+  <si>
+    <t>0.3767±0.011</t>
+  </si>
+  <si>
+    <t>0.109±0.0284</t>
+  </si>
+  <si>
+    <t>0.5926±0.0208</t>
+  </si>
+  <si>
+    <t>0.4005±0.0192</t>
   </si>
 </sst>
 </file>
@@ -6187,7 +7510,7 @@
   <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:N14"/>
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6242,60 +7565,492 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B3" t="s">
+        <v>1354</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1355</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1356</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1357</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1358</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1359</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1354</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1355</v>
+      </c>
+      <c r="K3" t="s">
+        <v>1356</v>
+      </c>
+      <c r="L3" t="s">
+        <v>1357</v>
+      </c>
+      <c r="M3" t="s">
+        <v>1358</v>
+      </c>
+      <c r="N3" t="s">
+        <v>1359</v>
+      </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B4" t="s">
+        <v>1354</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1355</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1356</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1357</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1358</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1359</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1354</v>
+      </c>
+      <c r="J4" t="s">
+        <v>1355</v>
+      </c>
+      <c r="K4" t="s">
+        <v>1356</v>
+      </c>
+      <c r="L4" t="s">
+        <v>1357</v>
+      </c>
+      <c r="M4" t="s">
+        <v>1358</v>
+      </c>
+      <c r="N4" t="s">
+        <v>1359</v>
+      </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B5" t="s">
+        <v>1354</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1355</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1356</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1357</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1358</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1359</v>
+      </c>
+      <c r="I5" t="s">
+        <v>1354</v>
+      </c>
+      <c r="J5" t="s">
+        <v>1355</v>
+      </c>
+      <c r="K5" t="s">
+        <v>1356</v>
+      </c>
+      <c r="L5" t="s">
+        <v>1357</v>
+      </c>
+      <c r="M5" t="s">
+        <v>1358</v>
+      </c>
+      <c r="N5" t="s">
+        <v>1359</v>
+      </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B6" t="s">
+        <v>1354</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1355</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1356</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1357</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1358</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1359</v>
+      </c>
+      <c r="I6" t="s">
+        <v>1354</v>
+      </c>
+      <c r="J6" t="s">
+        <v>1355</v>
+      </c>
+      <c r="K6" t="s">
+        <v>1356</v>
+      </c>
+      <c r="L6" t="s">
+        <v>1357</v>
+      </c>
+      <c r="M6" t="s">
+        <v>1358</v>
+      </c>
+      <c r="N6" t="s">
+        <v>1359</v>
+      </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B7" t="s">
+        <v>1354</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1355</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1356</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1357</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1358</v>
+      </c>
+      <c r="G7" t="s">
+        <v>1359</v>
+      </c>
+      <c r="I7" t="s">
+        <v>1354</v>
+      </c>
+      <c r="J7" t="s">
+        <v>1355</v>
+      </c>
+      <c r="K7" t="s">
+        <v>1356</v>
+      </c>
+      <c r="L7" t="s">
+        <v>1357</v>
+      </c>
+      <c r="M7" t="s">
+        <v>1358</v>
+      </c>
+      <c r="N7" t="s">
+        <v>1359</v>
+      </c>
     </row>
     <row r="8" spans="1:14" s="3" customFormat="1">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="B8" t="s">
+        <v>1354</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1355</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1356</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1357</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1358</v>
+      </c>
+      <c r="G8" t="s">
+        <v>1359</v>
+      </c>
+      <c r="I8" t="s">
+        <v>1354</v>
+      </c>
+      <c r="J8" t="s">
+        <v>1355</v>
+      </c>
+      <c r="K8" t="s">
+        <v>1356</v>
+      </c>
+      <c r="L8" t="s">
+        <v>1357</v>
+      </c>
+      <c r="M8" t="s">
+        <v>1358</v>
+      </c>
+      <c r="N8" t="s">
+        <v>1359</v>
+      </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B9" t="s">
+        <v>1354</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1355</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1356</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1357</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1358</v>
+      </c>
+      <c r="G9" t="s">
+        <v>1359</v>
+      </c>
+      <c r="I9" t="s">
+        <v>1354</v>
+      </c>
+      <c r="J9" t="s">
+        <v>1355</v>
+      </c>
+      <c r="K9" t="s">
+        <v>1356</v>
+      </c>
+      <c r="L9" t="s">
+        <v>1357</v>
+      </c>
+      <c r="M9" t="s">
+        <v>1358</v>
+      </c>
+      <c r="N9" t="s">
+        <v>1359</v>
+      </c>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B10" t="s">
+        <v>1354</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1355</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1356</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1357</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1358</v>
+      </c>
+      <c r="G10" t="s">
+        <v>1359</v>
+      </c>
+      <c r="I10" t="s">
+        <v>1354</v>
+      </c>
+      <c r="J10" t="s">
+        <v>1355</v>
+      </c>
+      <c r="K10" t="s">
+        <v>1356</v>
+      </c>
+      <c r="L10" t="s">
+        <v>1357</v>
+      </c>
+      <c r="M10" t="s">
+        <v>1358</v>
+      </c>
+      <c r="N10" t="s">
+        <v>1359</v>
+      </c>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B11" t="s">
+        <v>1354</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1355</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1356</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1357</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1358</v>
+      </c>
+      <c r="G11" t="s">
+        <v>1359</v>
+      </c>
+      <c r="I11" t="s">
+        <v>1360</v>
+      </c>
+      <c r="J11" t="s">
+        <v>1361</v>
+      </c>
+      <c r="K11" t="s">
+        <v>1356</v>
+      </c>
+      <c r="L11" t="s">
+        <v>1357</v>
+      </c>
+      <c r="M11" t="s">
+        <v>1358</v>
+      </c>
+      <c r="N11" t="s">
+        <v>1362</v>
+      </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="B12" t="s">
+        <v>1354</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1355</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1356</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1357</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1358</v>
+      </c>
+      <c r="G12" t="s">
+        <v>1359</v>
+      </c>
+      <c r="I12" t="s">
+        <v>1354</v>
+      </c>
+      <c r="J12" t="s">
+        <v>1355</v>
+      </c>
+      <c r="K12" t="s">
+        <v>1356</v>
+      </c>
+      <c r="L12" t="s">
+        <v>1357</v>
+      </c>
+      <c r="M12" t="s">
+        <v>1358</v>
+      </c>
+      <c r="N12" t="s">
+        <v>1359</v>
+      </c>
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="B13" t="s">
+        <v>1354</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1355</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1356</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1357</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1358</v>
+      </c>
+      <c r="G13" t="s">
+        <v>1359</v>
+      </c>
+      <c r="I13" t="s">
+        <v>1354</v>
+      </c>
+      <c r="J13" t="s">
+        <v>1355</v>
+      </c>
+      <c r="K13" t="s">
+        <v>1356</v>
+      </c>
+      <c r="L13" t="s">
+        <v>1357</v>
+      </c>
+      <c r="M13" t="s">
+        <v>1358</v>
+      </c>
+      <c r="N13" t="s">
+        <v>1359</v>
+      </c>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1354</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1355</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1356</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1357</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1358</v>
+      </c>
+      <c r="G14" t="s">
+        <v>1359</v>
+      </c>
+      <c r="I14" t="s">
+        <v>1354</v>
+      </c>
+      <c r="J14" t="s">
+        <v>1355</v>
+      </c>
+      <c r="K14" t="s">
+        <v>1356</v>
+      </c>
+      <c r="L14" t="s">
+        <v>1357</v>
+      </c>
+      <c r="M14" t="s">
+        <v>1358</v>
+      </c>
+      <c r="N14" t="s">
+        <v>1359</v>
       </c>
     </row>
     <row r="16" spans="1:14">
@@ -6354,8 +8109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3295008-3AAD-4E89-BA77-04BE8FBA0B66}">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:N14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6410,73 +8165,493 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B3" t="s">
+        <v>1651</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1652</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1653</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1654</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1655</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1656</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1723</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1724</v>
+      </c>
+      <c r="K3" t="s">
+        <v>1725</v>
+      </c>
+      <c r="L3" t="s">
+        <v>1726</v>
+      </c>
+      <c r="M3" t="s">
+        <v>1727</v>
+      </c>
+      <c r="N3" t="s">
+        <v>1728</v>
+      </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B4" t="s">
+        <v>1657</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1658</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1659</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1660</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1661</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1662</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1729</v>
+      </c>
+      <c r="J4" t="s">
+        <v>1730</v>
+      </c>
+      <c r="K4" t="s">
+        <v>1731</v>
+      </c>
+      <c r="L4" t="s">
+        <v>1732</v>
+      </c>
+      <c r="M4" t="s">
+        <v>1733</v>
+      </c>
+      <c r="N4" t="s">
+        <v>1734</v>
+      </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B5" t="s">
+        <v>1663</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1664</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1665</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1666</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1667</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1668</v>
+      </c>
+      <c r="I5" t="s">
+        <v>1735</v>
+      </c>
+      <c r="J5" t="s">
+        <v>1736</v>
+      </c>
+      <c r="K5" t="s">
+        <v>1737</v>
+      </c>
+      <c r="L5" t="s">
+        <v>1738</v>
+      </c>
+      <c r="M5" t="s">
+        <v>1739</v>
+      </c>
+      <c r="N5" t="s">
+        <v>1740</v>
+      </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B6" t="s">
+        <v>1669</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1670</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1671</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1672</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1673</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1674</v>
+      </c>
+      <c r="I6" t="s">
+        <v>1741</v>
+      </c>
+      <c r="J6" t="s">
+        <v>1742</v>
+      </c>
+      <c r="K6" t="s">
+        <v>1743</v>
+      </c>
+      <c r="L6" t="s">
+        <v>1744</v>
+      </c>
+      <c r="M6" t="s">
+        <v>1745</v>
+      </c>
+      <c r="N6" t="s">
+        <v>1746</v>
+      </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B7" t="s">
+        <v>1675</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1676</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1678</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1679</v>
+      </c>
+      <c r="G7" t="s">
+        <v>1680</v>
+      </c>
+      <c r="I7" t="s">
+        <v>1747</v>
+      </c>
+      <c r="J7" t="s">
+        <v>1748</v>
+      </c>
+      <c r="K7" t="s">
+        <v>1749</v>
+      </c>
+      <c r="L7" t="s">
+        <v>1750</v>
+      </c>
+      <c r="M7" t="s">
+        <v>1751</v>
+      </c>
+      <c r="N7" t="s">
+        <v>1752</v>
+      </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+      <c r="B8" t="s">
+        <v>1681</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1682</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1683</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1684</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1685</v>
+      </c>
+      <c r="G8" t="s">
+        <v>1686</v>
+      </c>
       <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
+      <c r="I8" t="s">
+        <v>1753</v>
+      </c>
+      <c r="J8" t="s">
+        <v>1754</v>
+      </c>
+      <c r="K8" t="s">
+        <v>1755</v>
+      </c>
+      <c r="L8" t="s">
+        <v>1756</v>
+      </c>
+      <c r="M8" t="s">
+        <v>1757</v>
+      </c>
+      <c r="N8" t="s">
+        <v>1758</v>
+      </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B9" t="s">
+        <v>1687</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1688</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1689</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1690</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1691</v>
+      </c>
+      <c r="G9" t="s">
+        <v>1692</v>
+      </c>
+      <c r="I9" t="s">
+        <v>1759</v>
+      </c>
+      <c r="J9" t="s">
+        <v>1760</v>
+      </c>
+      <c r="K9" t="s">
+        <v>1761</v>
+      </c>
+      <c r="L9" t="s">
+        <v>1762</v>
+      </c>
+      <c r="M9" t="s">
+        <v>1763</v>
+      </c>
+      <c r="N9" t="s">
+        <v>1764</v>
+      </c>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B10" t="s">
+        <v>1693</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1694</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1695</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1696</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1697</v>
+      </c>
+      <c r="G10" t="s">
+        <v>1698</v>
+      </c>
+      <c r="I10" t="s">
+        <v>1765</v>
+      </c>
+      <c r="J10" t="s">
+        <v>1766</v>
+      </c>
+      <c r="K10" t="s">
+        <v>1767</v>
+      </c>
+      <c r="L10" t="s">
+        <v>1768</v>
+      </c>
+      <c r="M10" t="s">
+        <v>1769</v>
+      </c>
+      <c r="N10" t="s">
+        <v>1770</v>
+      </c>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B11" t="s">
+        <v>1699</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1700</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1701</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1702</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1703</v>
+      </c>
+      <c r="G11" t="s">
+        <v>1704</v>
+      </c>
+      <c r="I11" t="s">
+        <v>1771</v>
+      </c>
+      <c r="J11" t="s">
+        <v>1772</v>
+      </c>
+      <c r="K11" t="s">
+        <v>1773</v>
+      </c>
+      <c r="L11" t="s">
+        <v>1774</v>
+      </c>
+      <c r="M11" t="s">
+        <v>1775</v>
+      </c>
+      <c r="N11" t="s">
+        <v>1776</v>
+      </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="B12" t="s">
+        <v>1705</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1706</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1707</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1708</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1709</v>
+      </c>
+      <c r="G12" t="s">
+        <v>1710</v>
+      </c>
+      <c r="I12" t="s">
+        <v>1777</v>
+      </c>
+      <c r="J12" t="s">
+        <v>1778</v>
+      </c>
+      <c r="K12" t="s">
+        <v>1779</v>
+      </c>
+      <c r="L12" t="s">
+        <v>1780</v>
+      </c>
+      <c r="M12" t="s">
+        <v>1781</v>
+      </c>
+      <c r="N12" t="s">
+        <v>1782</v>
+      </c>
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="B13" t="s">
+        <v>1711</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1712</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1713</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1714</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1715</v>
+      </c>
+      <c r="G13" t="s">
+        <v>1716</v>
+      </c>
+      <c r="I13" t="s">
+        <v>1783</v>
+      </c>
+      <c r="J13" t="s">
+        <v>1784</v>
+      </c>
+      <c r="K13" t="s">
+        <v>1785</v>
+      </c>
+      <c r="L13" t="s">
+        <v>1786</v>
+      </c>
+      <c r="M13" t="s">
+        <v>1787</v>
+      </c>
+      <c r="N13" t="s">
+        <v>1788</v>
+      </c>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1717</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1718</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1719</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1721</v>
+      </c>
+      <c r="G14" t="s">
+        <v>1722</v>
+      </c>
+      <c r="I14" t="s">
+        <v>1789</v>
+      </c>
+      <c r="J14" t="s">
+        <v>1790</v>
+      </c>
+      <c r="K14" t="s">
+        <v>1791</v>
+      </c>
+      <c r="L14" t="s">
+        <v>1792</v>
+      </c>
+      <c r="M14" t="s">
+        <v>1793</v>
+      </c>
+      <c r="N14" t="s">
+        <v>1794</v>
       </c>
     </row>
   </sheetData>
@@ -6489,7 +8664,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:N14"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6544,73 +8719,493 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B3" t="s">
+        <v>1363</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1364</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1365</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1366</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1367</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1368</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1435</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1436</v>
+      </c>
+      <c r="K3" t="s">
+        <v>1437</v>
+      </c>
+      <c r="L3" t="s">
+        <v>1438</v>
+      </c>
+      <c r="M3" t="s">
+        <v>1439</v>
+      </c>
+      <c r="N3" t="s">
+        <v>1440</v>
+      </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B4" t="s">
+        <v>1369</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1371</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1372</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1373</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1374</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1441</v>
+      </c>
+      <c r="J4" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K4" t="s">
+        <v>1443</v>
+      </c>
+      <c r="L4" t="s">
+        <v>1444</v>
+      </c>
+      <c r="M4" t="s">
+        <v>1445</v>
+      </c>
+      <c r="N4" t="s">
+        <v>1446</v>
+      </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B5" t="s">
+        <v>1375</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1376</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1377</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1378</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1379</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1380</v>
+      </c>
+      <c r="I5" t="s">
+        <v>1447</v>
+      </c>
+      <c r="J5" t="s">
+        <v>1448</v>
+      </c>
+      <c r="K5" t="s">
+        <v>1449</v>
+      </c>
+      <c r="L5" t="s">
+        <v>1450</v>
+      </c>
+      <c r="M5" t="s">
+        <v>1451</v>
+      </c>
+      <c r="N5" t="s">
+        <v>1452</v>
+      </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B6" t="s">
+        <v>1381</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1382</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1384</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1385</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1386</v>
+      </c>
+      <c r="I6" t="s">
+        <v>1453</v>
+      </c>
+      <c r="J6" t="s">
+        <v>1454</v>
+      </c>
+      <c r="K6" t="s">
+        <v>1455</v>
+      </c>
+      <c r="L6" t="s">
+        <v>1456</v>
+      </c>
+      <c r="M6" t="s">
+        <v>1457</v>
+      </c>
+      <c r="N6" t="s">
+        <v>1458</v>
+      </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B7" t="s">
+        <v>1387</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1388</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1389</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1390</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1391</v>
+      </c>
+      <c r="G7" t="s">
+        <v>1392</v>
+      </c>
+      <c r="I7" t="s">
+        <v>1459</v>
+      </c>
+      <c r="J7" t="s">
+        <v>1460</v>
+      </c>
+      <c r="K7" t="s">
+        <v>1461</v>
+      </c>
+      <c r="L7" t="s">
+        <v>1462</v>
+      </c>
+      <c r="M7" t="s">
+        <v>1463</v>
+      </c>
+      <c r="N7" t="s">
+        <v>1464</v>
+      </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+      <c r="B8" t="s">
+        <v>1393</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1395</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1396</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1397</v>
+      </c>
+      <c r="G8" t="s">
+        <v>1398</v>
+      </c>
       <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
+      <c r="I8" t="s">
+        <v>1465</v>
+      </c>
+      <c r="J8" t="s">
+        <v>1466</v>
+      </c>
+      <c r="K8" t="s">
+        <v>1467</v>
+      </c>
+      <c r="L8" t="s">
+        <v>1468</v>
+      </c>
+      <c r="M8" t="s">
+        <v>1469</v>
+      </c>
+      <c r="N8" t="s">
+        <v>1470</v>
+      </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B9" t="s">
+        <v>1399</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1400</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1401</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1402</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1403</v>
+      </c>
+      <c r="G9" t="s">
+        <v>1404</v>
+      </c>
+      <c r="I9" t="s">
+        <v>1471</v>
+      </c>
+      <c r="J9" t="s">
+        <v>1472</v>
+      </c>
+      <c r="K9" t="s">
+        <v>1473</v>
+      </c>
+      <c r="L9" t="s">
+        <v>1474</v>
+      </c>
+      <c r="M9" t="s">
+        <v>1475</v>
+      </c>
+      <c r="N9" t="s">
+        <v>1476</v>
+      </c>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B10" t="s">
+        <v>1405</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1406</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1407</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1408</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1409</v>
+      </c>
+      <c r="G10" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I10" t="s">
+        <v>1477</v>
+      </c>
+      <c r="J10" t="s">
+        <v>1478</v>
+      </c>
+      <c r="K10" t="s">
+        <v>1479</v>
+      </c>
+      <c r="L10" t="s">
+        <v>1480</v>
+      </c>
+      <c r="M10" t="s">
+        <v>1481</v>
+      </c>
+      <c r="N10" t="s">
+        <v>1482</v>
+      </c>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B11" t="s">
+        <v>1411</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1412</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1413</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1414</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1415</v>
+      </c>
+      <c r="G11" t="s">
+        <v>1416</v>
+      </c>
+      <c r="I11" t="s">
+        <v>1483</v>
+      </c>
+      <c r="J11" t="s">
+        <v>1484</v>
+      </c>
+      <c r="K11" t="s">
+        <v>1485</v>
+      </c>
+      <c r="L11" t="s">
+        <v>1486</v>
+      </c>
+      <c r="M11" t="s">
+        <v>1487</v>
+      </c>
+      <c r="N11" t="s">
+        <v>1488</v>
+      </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="B12" t="s">
+        <v>1417</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1418</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1419</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1420</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1421</v>
+      </c>
+      <c r="G12" t="s">
+        <v>1422</v>
+      </c>
+      <c r="I12" t="s">
+        <v>1489</v>
+      </c>
+      <c r="J12" t="s">
+        <v>1490</v>
+      </c>
+      <c r="K12" t="s">
+        <v>1491</v>
+      </c>
+      <c r="L12" t="s">
+        <v>1492</v>
+      </c>
+      <c r="M12" t="s">
+        <v>1493</v>
+      </c>
+      <c r="N12" t="s">
+        <v>1494</v>
+      </c>
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="B13" t="s">
+        <v>1423</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1424</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1425</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1426</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1427</v>
+      </c>
+      <c r="G13" t="s">
+        <v>1428</v>
+      </c>
+      <c r="I13" t="s">
+        <v>1495</v>
+      </c>
+      <c r="J13" t="s">
+        <v>1496</v>
+      </c>
+      <c r="K13" t="s">
+        <v>1497</v>
+      </c>
+      <c r="L13" t="s">
+        <v>1498</v>
+      </c>
+      <c r="M13" t="s">
+        <v>1499</v>
+      </c>
+      <c r="N13" t="s">
+        <v>1500</v>
+      </c>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1429</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1430</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1431</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1432</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1433</v>
+      </c>
+      <c r="G14" t="s">
+        <v>1434</v>
+      </c>
+      <c r="I14" t="s">
+        <v>1501</v>
+      </c>
+      <c r="J14" t="s">
+        <v>1502</v>
+      </c>
+      <c r="K14" t="s">
+        <v>1503</v>
+      </c>
+      <c r="L14" t="s">
+        <v>1504</v>
+      </c>
+      <c r="M14" t="s">
+        <v>1505</v>
+      </c>
+      <c r="N14" t="s">
+        <v>1506</v>
       </c>
     </row>
   </sheetData>
@@ -6622,8 +9217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A0953B5-619C-4EFA-A4D9-2FCC751D70A8}">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:N14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6678,73 +9273,493 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B3" t="s">
+        <v>1507</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1509</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1510</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1511</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1512</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1579</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1580</v>
+      </c>
+      <c r="K3" t="s">
+        <v>1581</v>
+      </c>
+      <c r="L3" t="s">
+        <v>1582</v>
+      </c>
+      <c r="M3" t="s">
+        <v>1583</v>
+      </c>
+      <c r="N3" t="s">
+        <v>1584</v>
+      </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B4" t="s">
+        <v>1513</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1514</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1515</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1516</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1517</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1518</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1585</v>
+      </c>
+      <c r="J4" t="s">
+        <v>1586</v>
+      </c>
+      <c r="K4" t="s">
+        <v>1587</v>
+      </c>
+      <c r="L4" t="s">
+        <v>1588</v>
+      </c>
+      <c r="M4" t="s">
+        <v>1589</v>
+      </c>
+      <c r="N4" t="s">
+        <v>1590</v>
+      </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B5" t="s">
+        <v>1519</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1520</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1521</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1522</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1523</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1524</v>
+      </c>
+      <c r="I5" t="s">
+        <v>1591</v>
+      </c>
+      <c r="J5" t="s">
+        <v>1592</v>
+      </c>
+      <c r="K5" t="s">
+        <v>1593</v>
+      </c>
+      <c r="L5" t="s">
+        <v>1594</v>
+      </c>
+      <c r="M5" t="s">
+        <v>1595</v>
+      </c>
+      <c r="N5" t="s">
+        <v>1596</v>
+      </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B6" t="s">
+        <v>1525</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1526</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1527</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1528</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1529</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1530</v>
+      </c>
+      <c r="I6" t="s">
+        <v>1597</v>
+      </c>
+      <c r="J6" t="s">
+        <v>1598</v>
+      </c>
+      <c r="K6" t="s">
+        <v>1599</v>
+      </c>
+      <c r="L6" t="s">
+        <v>1600</v>
+      </c>
+      <c r="M6" t="s">
+        <v>1601</v>
+      </c>
+      <c r="N6" t="s">
+        <v>1602</v>
+      </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B7" t="s">
+        <v>1531</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1532</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1533</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1534</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1535</v>
+      </c>
+      <c r="G7" t="s">
+        <v>1536</v>
+      </c>
+      <c r="I7" t="s">
+        <v>1603</v>
+      </c>
+      <c r="J7" t="s">
+        <v>1604</v>
+      </c>
+      <c r="K7" t="s">
+        <v>1605</v>
+      </c>
+      <c r="L7" t="s">
+        <v>1606</v>
+      </c>
+      <c r="M7" t="s">
+        <v>1607</v>
+      </c>
+      <c r="N7" t="s">
+        <v>1608</v>
+      </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+      <c r="B8" t="s">
+        <v>1537</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1538</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1539</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1540</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1541</v>
+      </c>
+      <c r="G8" t="s">
+        <v>1542</v>
+      </c>
       <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
+      <c r="I8" t="s">
+        <v>1609</v>
+      </c>
+      <c r="J8" t="s">
+        <v>1610</v>
+      </c>
+      <c r="K8" t="s">
+        <v>1611</v>
+      </c>
+      <c r="L8" t="s">
+        <v>1612</v>
+      </c>
+      <c r="M8" t="s">
+        <v>1613</v>
+      </c>
+      <c r="N8" t="s">
+        <v>1614</v>
+      </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B9" t="s">
+        <v>1543</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1544</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1545</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1546</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1547</v>
+      </c>
+      <c r="G9" t="s">
+        <v>1548</v>
+      </c>
+      <c r="I9" t="s">
+        <v>1615</v>
+      </c>
+      <c r="J9" t="s">
+        <v>1616</v>
+      </c>
+      <c r="K9" t="s">
+        <v>1617</v>
+      </c>
+      <c r="L9" t="s">
+        <v>1618</v>
+      </c>
+      <c r="M9" t="s">
+        <v>1619</v>
+      </c>
+      <c r="N9" t="s">
+        <v>1620</v>
+      </c>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B10" t="s">
+        <v>1549</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1550</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1551</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1552</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1553</v>
+      </c>
+      <c r="G10" t="s">
+        <v>1554</v>
+      </c>
+      <c r="I10" t="s">
+        <v>1621</v>
+      </c>
+      <c r="J10" t="s">
+        <v>1622</v>
+      </c>
+      <c r="K10" t="s">
+        <v>1623</v>
+      </c>
+      <c r="L10" t="s">
+        <v>1624</v>
+      </c>
+      <c r="M10" t="s">
+        <v>1625</v>
+      </c>
+      <c r="N10" t="s">
+        <v>1626</v>
+      </c>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B11" t="s">
+        <v>1555</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1556</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1557</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1558</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1559</v>
+      </c>
+      <c r="G11" t="s">
+        <v>1560</v>
+      </c>
+      <c r="I11" t="s">
+        <v>1627</v>
+      </c>
+      <c r="J11" t="s">
+        <v>1628</v>
+      </c>
+      <c r="K11" t="s">
+        <v>1629</v>
+      </c>
+      <c r="L11" t="s">
+        <v>1630</v>
+      </c>
+      <c r="M11" t="s">
+        <v>1631</v>
+      </c>
+      <c r="N11" t="s">
+        <v>1632</v>
+      </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="B12" t="s">
+        <v>1561</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1562</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1563</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1564</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1565</v>
+      </c>
+      <c r="G12" t="s">
+        <v>1566</v>
+      </c>
+      <c r="I12" t="s">
+        <v>1633</v>
+      </c>
+      <c r="J12" t="s">
+        <v>1634</v>
+      </c>
+      <c r="K12" t="s">
+        <v>1635</v>
+      </c>
+      <c r="L12" t="s">
+        <v>1636</v>
+      </c>
+      <c r="M12" t="s">
+        <v>1637</v>
+      </c>
+      <c r="N12" t="s">
+        <v>1638</v>
+      </c>
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="B13" t="s">
+        <v>1567</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1568</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1569</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1570</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1571</v>
+      </c>
+      <c r="G13" t="s">
+        <v>1572</v>
+      </c>
+      <c r="I13" t="s">
+        <v>1639</v>
+      </c>
+      <c r="J13" t="s">
+        <v>1640</v>
+      </c>
+      <c r="K13" t="s">
+        <v>1641</v>
+      </c>
+      <c r="L13" t="s">
+        <v>1642</v>
+      </c>
+      <c r="M13" t="s">
+        <v>1643</v>
+      </c>
+      <c r="N13" t="s">
+        <v>1644</v>
+      </c>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1573</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1574</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1575</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1576</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1577</v>
+      </c>
+      <c r="G14" t="s">
+        <v>1578</v>
+      </c>
+      <c r="I14" t="s">
+        <v>1645</v>
+      </c>
+      <c r="J14" t="s">
+        <v>1646</v>
+      </c>
+      <c r="K14" t="s">
+        <v>1647</v>
+      </c>
+      <c r="L14" t="s">
+        <v>1648</v>
+      </c>
+      <c r="M14" t="s">
+        <v>1649</v>
+      </c>
+      <c r="N14" t="s">
+        <v>1650</v>
       </c>
     </row>
   </sheetData>

</xml_diff>